<commit_message>
Système de comparaison des centres VHU et tri de ceux-ci -> On met dans un fichier Excel les centres VHU qui n'existent pas dans la BDD
</commit_message>
<xml_diff>
--- a/uploads/Tables Syderep_V4.xlsx
+++ b/uploads/Tables Syderep_V4.xlsx
@@ -2543,7 +2543,7 @@
     <t>VER</t>
   </si>
   <si>
-    <t>Tables Syderep_V4  2017-02-27 14:03:21</t>
+    <t>Tables Syderep_V4  2017-02-27 18:05:55</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -2896,7 +2896,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2968,6 +2968,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF79646"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF3498DB"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -3026,7 +3032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3170,12 +3176,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3194,10 +3194,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3516,7 +3519,7 @@
     <col min="7" max="7" width="51.140625" style="48" customWidth="1"/>
     <col min="8" max="8" width="51.140625" style="47" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="47" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="52"/>
+    <col min="10" max="10" width="9.140625" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3545,7 +3548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>8</v>
       </c>
@@ -3567,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>13</v>
       </c>
@@ -3591,7 +3594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>18</v>
       </c>
@@ -3997,7 +4000,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="53" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
         <v>80</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>93</v>
       </c>
@@ -4429,7 +4432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>141</v>
       </c>
@@ -4597,7 +4600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
         <v>166</v>
       </c>
@@ -4811,7 +4814,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
         <v>191</v>
       </c>
@@ -5077,7 +5080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="31" t="s">
         <v>230</v>
       </c>
@@ -5295,7 +5298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="31" t="s">
         <v>259</v>
       </c>
@@ -5705,7 +5708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="31" t="s">
         <v>312</v>
       </c>
@@ -5753,7 +5756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="31" t="s">
         <v>318</v>
       </c>
@@ -5777,7 +5780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="31" t="s">
         <v>321</v>
       </c>
@@ -5801,7 +5804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="31" t="s">
         <v>325</v>
       </c>
@@ -5825,7 +5828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="31" t="s">
         <v>328</v>
       </c>
@@ -5849,7 +5852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="31" t="s">
         <v>331</v>
       </c>
@@ -5897,7 +5900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="31" t="s">
         <v>339</v>
       </c>
@@ -5921,7 +5924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="31" t="s">
         <v>342</v>
       </c>
@@ -5945,7 +5948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="31" t="s">
         <v>345</v>
       </c>
@@ -5971,7 +5974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="31" t="s">
         <v>348</v>
       </c>
@@ -5997,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="31" t="s">
         <v>351</v>
       </c>
@@ -6021,7 +6024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="31" t="s">
         <v>355</v>
       </c>
@@ -6069,7 +6072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="31" t="s">
         <v>361</v>
       </c>
@@ -6093,7 +6096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="31" t="s">
         <v>365</v>
       </c>
@@ -6117,7 +6120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="31" t="s">
         <v>368</v>
       </c>
@@ -6165,7 +6168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="31" t="s">
         <v>374</v>
       </c>
@@ -6189,7 +6192,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="31" t="s">
         <v>376</v>
       </c>
@@ -6215,7 +6218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="31" t="s">
         <v>378</v>
       </c>
@@ -6239,7 +6242,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="31" t="s">
         <v>380</v>
       </c>
@@ -6263,7 +6266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="115" spans="1:8" s="54" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" s="52" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="39" t="s">
         <v>382</v>
       </c>
@@ -6311,7 +6314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="31" t="s">
         <v>389</v>
       </c>
@@ -6335,7 +6338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="31" t="s">
         <v>393</v>
       </c>
@@ -6359,7 +6362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="31" t="s">
         <v>397</v>
       </c>
@@ -6381,7 +6384,7 @@
       <c r="G119" s="31"/>
       <c r="H119" s="19"/>
     </row>
-    <row r="120" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="31" t="s">
         <v>400</v>
       </c>
@@ -6405,7 +6408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="31" t="s">
         <v>404</v>
       </c>
@@ -6429,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="31" t="s">
         <v>408</v>
       </c>
@@ -6477,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="31" t="s">
         <v>414</v>
       </c>
@@ -6501,7 +6504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="31" t="s">
         <v>417</v>
       </c>
@@ -6525,7 +6528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="31" t="s">
         <v>420</v>
       </c>
@@ -6547,7 +6550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="31" t="s">
         <v>422</v>
       </c>
@@ -6571,7 +6574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="31" t="s">
         <v>425</v>
       </c>
@@ -7099,7 +7102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="31" t="s">
         <v>493</v>
       </c>
@@ -7147,7 +7150,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="152" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="31" t="s">
         <v>499</v>
       </c>
@@ -7317,7 +7320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="31" t="s">
         <v>521</v>
       </c>
@@ -7509,7 +7512,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="167" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="31" t="s">
         <v>545</v>
       </c>
@@ -7533,7 +7536,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="168" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="31" t="s">
         <v>547</v>
       </c>
@@ -7559,7 +7562,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="169" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="31" t="s">
         <v>549</v>
       </c>
@@ -7583,7 +7586,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="31" t="s">
         <v>551</v>
       </c>
@@ -7607,7 +7610,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="171" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="31" t="s">
         <v>553</v>
       </c>
@@ -7703,7 +7706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="31" t="s">
         <v>563</v>
       </c>
@@ -7821,7 +7824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="31" t="s">
         <v>575</v>
       </c>
@@ -7847,7 +7850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="31" t="s">
         <v>578</v>
       </c>
@@ -7897,7 +7900,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="183" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="31" t="s">
         <v>582</v>
       </c>
@@ -7945,7 +7948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="31" t="s">
         <v>588</v>
       </c>
@@ -7969,7 +7972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="31" t="s">
         <v>592</v>
       </c>
@@ -7993,7 +7996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="31" t="s">
         <v>596</v>
       </c>
@@ -8017,7 +8020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="31" t="s">
         <v>600</v>
       </c>
@@ -8089,7 +8092,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="191" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="31" t="s">
         <v>608</v>
       </c>
@@ -8113,7 +8116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="31" t="s">
         <v>611</v>
       </c>
@@ -8137,7 +8140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="31" t="s">
         <v>614</v>
       </c>
@@ -8185,7 +8188,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="31" t="s">
         <v>620</v>
       </c>
@@ -8329,7 +8332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="31" t="s">
         <v>634</v>
       </c>
@@ -8353,7 +8356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="31" t="s">
         <v>637</v>
       </c>
@@ -8403,7 +8406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="31" t="s">
         <v>643</v>
       </c>
@@ -8427,7 +8430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="31" t="s">
         <v>646</v>
       </c>
@@ -8475,7 +8478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="31" t="s">
         <v>652</v>
       </c>
@@ -8499,7 +8502,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="208" spans="1:8" s="51" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" s="49" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="31" t="s">
         <v>654</v>
       </c>
@@ -8525,7 +8528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="31" t="s">
         <v>658</v>
       </c>
@@ -8549,7 +8552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="31" t="s">
         <v>661</v>
       </c>
@@ -8573,7 +8576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="31" t="s">
         <v>664</v>
       </c>
@@ -8597,7 +8600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:8" s="51" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" s="49" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="31" t="s">
         <v>667</v>
       </c>
@@ -8761,7 +8764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="31" t="s">
         <v>686</v>
       </c>
@@ -8785,7 +8788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:8" s="51" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="33" t="s">
         <v>689</v>
       </c>
@@ -10222,89 +10225,104 @@
       </c>
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A295" s="49" t="s">
+      <c r="A295" s="55" t="s">
         <v>832</v>
       </c>
-      <c r="B295" s="45"/>
-      <c r="C295" s="45" t="s">
+      <c r="B295" s="7"/>
+      <c r="C295" s="7" t="s">
         <v>749</v>
       </c>
-      <c r="D295" s="45"/>
-      <c r="E295" s="45"/>
-      <c r="F295" s="45"/>
-      <c r="G295" s="46"/>
-      <c r="H295" s="41">
+      <c r="D295" s="7"/>
+      <c r="E295" s="7"/>
+      <c r="F295" s="7"/>
+      <c r="G295" s="43"/>
+      <c r="H295" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A296" s="50" t="s">
+      <c r="A296" s="55" t="s">
         <v>833</v>
       </c>
-      <c r="C296" s="47" t="s">
+      <c r="B296" s="7"/>
+      <c r="C296" s="7" t="s">
         <v>834</v>
       </c>
-      <c r="H296" s="41">
+      <c r="D296" s="7"/>
+      <c r="E296" s="7"/>
+      <c r="F296" s="7"/>
+      <c r="G296" s="43"/>
+      <c r="H296" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A297" s="50" t="s">
+      <c r="A297" s="55" t="s">
         <v>835</v>
       </c>
-      <c r="C297" s="47" t="s">
+      <c r="B297" s="7"/>
+      <c r="C297" s="7" t="s">
         <v>565</v>
       </c>
-      <c r="H297" s="41">
+      <c r="D297" s="7"/>
+      <c r="E297" s="7"/>
+      <c r="F297" s="7"/>
+      <c r="G297" s="43"/>
+      <c r="H297" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="298" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A298" s="50" t="s">
+      <c r="A298" s="55" t="s">
         <v>836</v>
       </c>
-      <c r="C298" s="47" t="s">
+      <c r="B298" s="7"/>
+      <c r="C298" s="7" t="s">
         <v>837</v>
       </c>
-      <c r="H298" s="41">
+      <c r="D298" s="7"/>
+      <c r="E298" s="7"/>
+      <c r="F298" s="7"/>
+      <c r="G298" s="43"/>
+      <c r="H298" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A299" s="57" t="s">
+      <c r="A299" s="56" t="s">
         <v>838</v>
       </c>
-      <c r="B299" s="57" t="s">
+      <c r="B299" s="56" t="s">
         <v>838</v>
       </c>
-      <c r="C299" s="57" t="s">
+      <c r="C299" s="56" t="s">
         <v>838</v>
       </c>
-      <c r="D299" s="57" t="s">
+      <c r="D299" s="56" t="s">
         <v>838</v>
       </c>
-      <c r="E299" s="57" t="s">
+      <c r="E299" s="56" t="s">
         <v>838</v>
       </c>
-      <c r="F299" s="57" t="s">
+      <c r="F299" s="56" t="s">
         <v>838</v>
       </c>
-      <c r="G299" s="58" t="s">
+      <c r="G299" s="57" t="s">
         <v>838</v>
       </c>
-      <c r="H299" s="57" t="s">
+      <c r="H299" s="56" t="s">
         <v>838</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A300" s="55"/>
-      <c r="B300" s="55"/>
-      <c r="C300" s="55"/>
-      <c r="D300" s="55"/>
-      <c r="E300" s="55"/>
-      <c r="F300" s="55"/>
-      <c r="G300" s="56"/>
-      <c r="H300" s="55"/>
+      <c r="A300" s="53"/>
+      <c r="B300" s="53"/>
+      <c r="C300" s="53"/>
+      <c r="D300" s="53"/>
+      <c r="E300" s="53"/>
+      <c r="F300" s="53"/>
+      <c r="G300" s="54"/>
+      <c r="H300" s="53"/>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C301" s="47" t="s">

</xml_diff>